<commit_message>
updated with DataProvider for validCode
</commit_message>
<xml_diff>
--- a/org.dsalgo/src/test/resources/testData/testData.xlsx
+++ b/org.dsalgo/src/test/resources/testData/testData.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\link2\git\dsalgo_ninjalinos-BDD\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7140CFB5-16FE-4B55-A330-29643202B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A998473A-40C6-4B26-937F-E92F5FD20BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TextEditor" sheetId="1" r:id="rId1"/>
+    <sheet name="Credentials" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,40 +22,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Valid Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Invalid Code </t>
-  </si>
-  <si>
-    <t>Actual Results</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Expected Results- Valid Code</t>
-  </si>
-  <si>
-    <t>Expected Results- Invalid Code</t>
-  </si>
-  <si>
-    <t>DsAlgoNew</t>
-  </si>
-  <si>
     <t>print("Hello World")</t>
   </si>
   <si>
-    <t>Hello World</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ninjalinos@work.com</t>
+  </si>
+  <si>
+    <t>sdet218920@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +58,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,17 +94,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,57 +386,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA50DD17-A988-4160-B951-9710869CC38D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8ABF38AF-820C-4478-9F1D-96065AE9D5A1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>